<commit_message>
new update for automatic calculation depending of the operator umbrella
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -8,22 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diop9188\PycharmProjects\DOIpallier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F422A-E3D2-484D-BB0D-97723CE7BCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2DC95-DC3E-4B3D-9784-0F1C93B9B839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$I$6</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Deal</t>
   </si>
@@ -58,6 +71,9 @@
     <t>libon</t>
   </si>
   <si>
+    <t>FT</t>
+  </si>
+  <si>
     <t>gap</t>
   </si>
   <si>
@@ -70,14 +86,37 @@
     <t>lyca</t>
   </si>
   <si>
+    <t>Belgacom</t>
+  </si>
+  <si>
     <t>ofr</t>
+  </si>
+  <si>
+    <t>usa/etail</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>China Corp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* ###0_-;\-* ###0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +142,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,11 +504,13 @@
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -518,21 +562,24 @@
         <v>3000000</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H2">
         <v>33</v>
       </c>
       <c r="I2">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="J2">
-        <v>50310916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>155187164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>66</v>
@@ -547,9 +594,9 @@
         <v>89602986</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>89</v>
@@ -564,9 +611,9 @@
         <v>29141537</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>151</v>
@@ -580,10 +627,13 @@
       <c r="J5">
         <v>15777537</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>289709224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -601,21 +651,24 @@
         <v>3000000</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H6">
         <v>33</v>
       </c>
       <c r="I6">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="J6">
-        <v>-15039328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>62128888</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>59</v>
@@ -628,10 +681,189 @@
       </c>
       <c r="J7">
         <v>50976000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>40000</v>
+      </c>
+      <c r="J8">
+        <v>2880000</v>
+      </c>
+      <c r="L8">
+        <v>115984888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>700000</v>
+      </c>
+      <c r="J9">
+        <v>55300000</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>1000000</v>
+      </c>
+      <c r="L11">
+        <v>57300000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f>J2+J3+J4+J5</f>
+        <v>289709224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>J6+J7+J8</f>
+        <v>115984888</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f>J9+J10+J11</f>
+        <v>57300000</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E4">
+        <v>52476560</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8312452</v>
+      </c>
+      <c r="E5">
+        <v>65595700.000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E6">
+        <v>34847400.765639998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>52.476559999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>32.797849999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.5595699999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>155187164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>